<commit_message>
Paul can have a nicer nickname
</commit_message>
<xml_diff>
--- a/static/downloads/2021/WMRRA-2021-Final-Points-09192021.xlsx
+++ b/static/downloads/2021/WMRRA-2021-Final-Points-09192021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crwilcox\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\crwilcox\workspace\wmrra-com\static\downloads\2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E535133-F5E2-48C4-8DDD-E1C4B1681D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E8B33B-FBD8-4991-9507-64C8D7F60C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="10044" xr2:uid="{58302ADD-EE14-46B2-B8AB-B8706E5B8C2C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{58302ADD-EE14-46B2-B8AB-B8706E5B8C2C}"/>
   </bookViews>
   <sheets>
     <sheet name="2021 Championship" sheetId="1" r:id="rId1"/>
@@ -620,15 +620,9 @@
     <t>Dave "Down Here" Pearce</t>
   </si>
   <si>
-    <t>Paul "StaysHomesy" McComsey</t>
-  </si>
-  <si>
     <t>Scott "Mr. Hair" Harris</t>
   </si>
   <si>
-    <t>Chris "Badger" Wilcox</t>
-  </si>
-  <si>
     <t>Joel "Pink's My Color" Ohman</t>
   </si>
   <si>
@@ -636,6 +630,12 @@
   </si>
   <si>
     <t>Seppi "T-Rex" Hutter</t>
+  </si>
+  <si>
+    <t>Paul "Racing's in the Rearview" McComsey</t>
+  </si>
+  <si>
+    <t>Chris "Bagel Badger" Wilcox</t>
   </si>
 </sst>
 </file>
@@ -2038,10 +2038,10 @@
   <dimension ref="A1:U109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C104" sqref="C104"/>
+      <selection pane="bottomRight" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3047,7 +3047,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="80" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D25" s="31"/>
       <c r="E25" s="140">
@@ -3722,7 +3722,7 @@
         <v>152</v>
       </c>
       <c r="C43" s="135" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
@@ -3838,7 +3838,7 @@
         <v>47</v>
       </c>
       <c r="C46" s="80" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D46" s="31"/>
       <c r="E46" s="31">
@@ -3983,7 +3983,7 @@
         <v>92</v>
       </c>
       <c r="C50" s="131" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D50" s="31"/>
       <c r="E50" s="30">
@@ -4450,7 +4450,7 @@
         <v>253</v>
       </c>
       <c r="C63" s="80" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D63" s="31"/>
       <c r="E63" s="140">
@@ -5428,7 +5428,7 @@
         <v>810</v>
       </c>
       <c r="C89" s="51" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D89" s="24"/>
       <c r="E89" s="24"/>

</xml_diff>